<commit_message>
#21 Updated registration feature test outputs picture and test case documentation
Test outputs and test case documentation has been updated after testing of registration page is completed.
</commit_message>
<xml_diff>
--- a/TestCases/Test Cases - Registration.xlsx
+++ b/TestCases/Test Cases - Registration.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zxlbm\Downloads\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Asus\Desktop\ETI_ToDoList\TestCases\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{80DCFB1F-DFBA-4254-BFCE-56FC333BCF22}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B8B16F1F-E037-4034-A4BD-E2D3EB485F5F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15810" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61" uniqueCount="42">
   <si>
     <t>Test Case Scenario</t>
   </si>
@@ -49,9 +49,6 @@
   </si>
   <si>
     <t>Fail/Pass</t>
-  </si>
-  <si>
-    <t>Fail</t>
   </si>
   <si>
     <t>-</t>
@@ -175,6 +172,12 @@
   </si>
   <si>
     <t>Registration attempt failed. User will be shown the requirements for the username field and prompted to come up with a username to meet the requirements.</t>
+  </si>
+  <si>
+    <t>Same as expected outcome.</t>
+  </si>
+  <si>
+    <t>Pass</t>
   </si>
 </sst>
 </file>
@@ -544,25 +547,25 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:G15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G4" sqref="G4"/>
+    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultColWidth="9.1796875" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="4.42578125" style="2" customWidth="1"/>
-    <col min="2" max="2" width="44.85546875" style="2" customWidth="1"/>
-    <col min="3" max="3" width="34.140625" style="2" customWidth="1"/>
-    <col min="4" max="4" width="58.7109375" style="2" customWidth="1"/>
-    <col min="5" max="5" width="27.7109375" style="2" customWidth="1"/>
-    <col min="6" max="7" width="17.42578125" style="2" customWidth="1"/>
-    <col min="8" max="8" width="17.28515625" style="2" customWidth="1"/>
-    <col min="9" max="16384" width="9.140625" style="2"/>
+    <col min="1" max="1" width="4.453125" style="2" customWidth="1"/>
+    <col min="2" max="2" width="44.81640625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="34.1796875" style="2" customWidth="1"/>
+    <col min="4" max="4" width="58.7265625" style="2" customWidth="1"/>
+    <col min="5" max="5" width="27.7265625" style="2" customWidth="1"/>
+    <col min="6" max="7" width="17.453125" style="2" customWidth="1"/>
+    <col min="8" max="8" width="17.26953125" style="2" customWidth="1"/>
+    <col min="9" max="16384" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:7" ht="15.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -583,214 +586,214 @@
         <v>5</v>
       </c>
     </row>
-    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:7" ht="61.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A2" s="5">
         <v>4</v>
       </c>
       <c r="B2" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="C2" s="6" t="s">
         <v>9</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="D2" s="6" t="s">
+        <v>6</v>
+      </c>
+      <c r="E2" s="6" t="s">
         <v>10</v>
       </c>
-      <c r="D2" s="6" t="s">
-        <v>7</v>
-      </c>
-      <c r="E2" s="6" t="s">
-        <v>11</v>
-      </c>
       <c r="F2" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G2" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="96" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A3" s="6">
         <v>4.0999999999999996</v>
       </c>
       <c r="B3" s="6" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="D3" s="6" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="E3" s="6" t="s">
+        <v>39</v>
+      </c>
+      <c r="F3" s="6" t="s">
         <v>40</v>
       </c>
-      <c r="F3" s="6" t="s">
-        <v>7</v>
-      </c>
       <c r="G3" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7" ht="62.45" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" ht="62.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A4" s="6">
         <v>4.2</v>
       </c>
       <c r="B4" s="6" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="D4" s="6" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="E4" s="6" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="F4" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G4" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="5" spans="1:7" ht="63.95" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" ht="64" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A5" s="6">
         <v>4.3</v>
       </c>
       <c r="B5" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="C5" s="6" t="s">
         <v>22</v>
       </c>
-      <c r="C5" s="6" t="s">
+      <c r="D5" s="6" t="s">
         <v>23</v>
       </c>
-      <c r="D5" s="6" t="s">
-        <v>24</v>
-      </c>
       <c r="E5" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F5" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G5" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" ht="64.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A6" s="6">
         <v>4.4000000000000004</v>
       </c>
       <c r="B6" s="6" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="D6" s="6" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="E6" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F6" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G6" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="7" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="67.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A7" s="6">
         <v>4.5</v>
       </c>
       <c r="B7" s="6" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="D7" s="6" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="E7" s="6" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="F7" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G7" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="72.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A8" s="6">
         <v>4.5999999999999996</v>
       </c>
       <c r="B8" s="6" t="s">
+        <v>31</v>
+      </c>
+      <c r="C8" s="6" t="s">
         <v>32</v>
       </c>
-      <c r="C8" s="6" t="s">
+      <c r="D8" s="6" t="s">
         <v>33</v>
       </c>
-      <c r="D8" s="6" t="s">
-        <v>34</v>
-      </c>
       <c r="E8" s="6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="F8" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G8" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" ht="57.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A9" s="6">
         <v>4.7</v>
       </c>
       <c r="B9" s="6" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="D9" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E9" s="6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="F9" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G9" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" ht="73.5" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A10" s="6">
         <v>4.8</v>
       </c>
       <c r="B10" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="C10" s="6" t="s">
         <v>19</v>
       </c>
-      <c r="C10" s="6" t="s">
-        <v>20</v>
-      </c>
       <c r="D10" s="6" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="E10" s="6" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="F10" s="6" t="s">
-        <v>7</v>
+        <v>40</v>
       </c>
       <c r="G10" s="6" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.25">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="60.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A11" s="3"/>
       <c r="B11" s="3"/>
       <c r="C11" s="3"/>
@@ -799,7 +802,7 @@
       <c r="F11" s="3"/>
       <c r="G11" s="3"/>
     </row>
-    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:7" ht="62.25" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A12" s="4"/>
       <c r="B12" s="3"/>
       <c r="C12" s="3"/>
@@ -808,7 +811,7 @@
       <c r="F12" s="3"/>
       <c r="G12" s="3"/>
     </row>
-    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:7" ht="57" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A13" s="3"/>
       <c r="B13" s="3"/>
       <c r="C13" s="3"/>
@@ -817,7 +820,7 @@
       <c r="F13" s="3"/>
       <c r="G13" s="3"/>
     </row>
-    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="51.75" customHeight="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3"/>
       <c r="B14" s="3"/>
       <c r="C14" s="3"/>
@@ -826,7 +829,7 @@
       <c r="F14" s="3"/>
       <c r="G14" s="3"/>
     </row>
-    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.25"/>
+    <row r="15" spans="1:7" ht="35.25" customHeight="1" x14ac:dyDescent="0.35"/>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>

</xml_diff>